<commit_message>
Revert "update indicator list"
This reverts commit fa39f96dc2e4fca720bdad9cb0f3587380ff198e.
</commit_message>
<xml_diff>
--- a/Cork_Dashboard_Indicator_List.xlsx
+++ b/Cork_Dashboard_Indicator_List.xlsx
@@ -1,29 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Documents/repos/bcd-cd-v2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skeogh\Documents\BuildingCityDashboards\Corkdashboard\Cork_indicators_data_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{359B2750-CEBD-490A-8587-66E6E2C83749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -495,8 +489,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,7 +580,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,58 +588,58 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -653,7 +647,7 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
@@ -662,35 +656,35 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -698,7 +692,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -1054,23 +1048,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView topLeftCell="D58" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="85.1640625" customWidth="1"/>
-    <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="211.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="211.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="45.75" customHeight="1">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1073,7 @@
       <c r="D1" s="55"/>
       <c r="E1" s="55"/>
     </row>
-    <row r="2" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="23.25" customHeight="1">
       <c r="A2" s="56" t="s">
         <v>1</v>
       </c>
@@ -1088,14 +1082,14 @@
       <c r="D2" s="56"/>
       <c r="E2" s="56"/>
     </row>
-    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="23.25" customHeight="1">
       <c r="A3" s="57"/>
       <c r="B3" s="57"/>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
       <c r="E3" s="57"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1112,7 +1106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1129,7 +1123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1146,7 +1140,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1157,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
         <v>18</v>
@@ -1178,7 +1172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="8"/>
       <c r="B9" s="10" t="s">
         <v>19</v>
@@ -1193,7 +1187,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="8"/>
       <c r="B10" s="10" t="s">
         <v>20</v>
@@ -1208,7 +1202,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="8"/>
       <c r="B11" s="10" t="s">
         <v>21</v>
@@ -1223,7 +1217,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="8"/>
       <c r="B12" s="10" t="s">
         <v>22</v>
@@ -1238,7 +1232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="11"/>
       <c r="B13" s="10" t="s">
         <v>24</v>
@@ -1253,7 +1247,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="11"/>
       <c r="B14" s="10" t="s">
         <v>27</v>
@@ -1268,7 +1262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="11"/>
       <c r="B15" s="10" t="s">
         <v>28</v>
@@ -1283,7 +1277,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="11"/>
       <c r="B16" s="10" t="s">
         <v>31</v>
@@ -1298,7 +1292,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="11"/>
       <c r="B17" s="12" t="s">
         <v>33</v>
@@ -1313,7 +1307,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="13" t="s">
         <v>35</v>
       </c>
@@ -1330,7 +1324,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="17" t="s">
         <v>39</v>
       </c>
@@ -1345,7 +1339,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="17" t="s">
         <v>41</v>
       </c>
@@ -1362,7 +1356,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14" t="s">
@@ -1375,7 +1369,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="14"/>
       <c r="B22" s="14" t="s">
         <v>43</v>
@@ -1390,7 +1384,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14" t="s">
@@ -1403,7 +1397,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="14"/>
       <c r="B24" s="14" t="s">
         <v>47</v>
@@ -1418,7 +1412,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14" t="s">
@@ -1431,7 +1425,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="14"/>
       <c r="B26" s="14" t="s">
         <v>51</v>
@@ -1446,7 +1440,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14" t="s">
@@ -1459,7 +1453,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14" t="s">
@@ -1472,7 +1466,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14" t="s">
@@ -1485,7 +1479,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" s="14"/>
       <c r="B30" s="14" t="s">
         <v>57</v>
@@ -1500,7 +1494,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14" t="s">
@@ -1513,7 +1507,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" s="14"/>
       <c r="B32" s="14" t="s">
         <v>62</v>
@@ -1528,7 +1522,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="21" t="s">
@@ -1541,7 +1535,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" s="23" t="s">
         <v>65</v>
       </c>
@@ -1558,7 +1552,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" s="27"/>
       <c r="B35" s="27"/>
       <c r="C35" s="25" t="s">
@@ -1571,7 +1565,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" s="27"/>
       <c r="B36" s="27" t="s">
         <v>68</v>
@@ -1586,7 +1580,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" s="27"/>
       <c r="B37" s="27"/>
       <c r="C37" s="25" t="s">
@@ -1599,7 +1593,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" s="27"/>
       <c r="B38" s="27" t="s">
         <v>69</v>
@@ -1614,7 +1608,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="27"/>
       <c r="B39" s="27"/>
       <c r="C39" s="25" t="s">
@@ -1627,7 +1621,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="27"/>
       <c r="B40" s="27" t="s">
         <v>71</v>
@@ -1642,7 +1636,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" s="27"/>
       <c r="B41" s="27"/>
       <c r="C41" s="25" t="s">
@@ -1655,7 +1649,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" s="27"/>
       <c r="B42" s="27" t="s">
         <v>73</v>
@@ -1670,7 +1664,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" s="27"/>
       <c r="B43" s="27"/>
       <c r="C43" s="25" t="s">
@@ -1683,7 +1677,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" s="27"/>
       <c r="B44" s="27" t="s">
         <v>75</v>
@@ -1698,7 +1692,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" s="27"/>
       <c r="B45" s="27"/>
       <c r="C45" s="25" t="s">
@@ -1711,7 +1705,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" s="28"/>
       <c r="B46" s="28" t="s">
         <v>77</v>
@@ -1726,7 +1720,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="27"/>
       <c r="B47" s="27" t="s">
         <v>80</v>
@@ -1741,7 +1735,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" s="27"/>
       <c r="B48" s="27" t="s">
         <v>83</v>
@@ -1756,7 +1750,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" s="27"/>
       <c r="B49" s="27" t="s">
         <v>84</v>
@@ -1771,7 +1765,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" s="27"/>
       <c r="B50" s="27"/>
       <c r="C50" s="25" t="s">
@@ -1784,7 +1778,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" s="29" t="s">
         <v>86</v>
       </c>
@@ -1801,7 +1795,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" s="33"/>
       <c r="B52" s="33" t="s">
         <v>89</v>
@@ -1816,7 +1810,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" s="33"/>
       <c r="B53" s="33" t="s">
         <v>90</v>
@@ -1831,7 +1825,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" s="33"/>
       <c r="B54" s="33" t="s">
         <v>92</v>
@@ -1846,7 +1840,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" s="33"/>
       <c r="B55" s="33" t="s">
         <v>94</v>
@@ -1861,7 +1855,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" s="33"/>
       <c r="B56" s="33" t="s">
         <v>96</v>
@@ -1876,7 +1870,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" s="33"/>
       <c r="B57" s="30" t="s">
         <v>97</v>
@@ -1891,7 +1885,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" s="34"/>
       <c r="B58" s="34"/>
       <c r="C58" s="31" t="s">
@@ -1904,7 +1898,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" s="33"/>
       <c r="B59" s="33"/>
       <c r="C59" s="31" t="s">
@@ -1917,7 +1911,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" s="33"/>
       <c r="B60" s="33" t="s">
         <v>99</v>
@@ -1932,7 +1926,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" s="33"/>
       <c r="B61" s="33"/>
       <c r="C61" s="31" t="s">
@@ -1945,7 +1939,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" s="35" t="s">
         <v>101</v>
       </c>
@@ -1962,7 +1956,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63" s="39" t="s">
         <v>105</v>
       </c>
@@ -1977,7 +1971,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64" s="42"/>
       <c r="B64" s="40" t="s">
         <v>107</v>
@@ -1992,7 +1986,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65" s="42"/>
       <c r="B65" s="41"/>
       <c r="C65" s="37" t="s">
@@ -2005,7 +1999,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5">
       <c r="A66" s="40"/>
       <c r="B66" s="36" t="s">
         <v>109</v>
@@ -2020,7 +2014,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67" s="40"/>
       <c r="B67" s="40"/>
       <c r="C67" s="37" t="s">
@@ -2033,7 +2027,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" s="40"/>
       <c r="B68" s="40" t="s">
         <v>111</v>
@@ -2048,7 +2042,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69" s="40"/>
       <c r="B69" s="40"/>
       <c r="C69" s="37" t="s">
@@ -2061,7 +2055,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70" s="40"/>
       <c r="B70" s="40" t="s">
         <v>112</v>
@@ -2076,7 +2070,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71" s="40"/>
       <c r="B71" s="40"/>
       <c r="C71" s="37" t="s">
@@ -2089,7 +2083,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72" s="40"/>
       <c r="B72" s="40" t="s">
         <v>113</v>
@@ -2104,7 +2098,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73" s="40"/>
       <c r="B73" s="40"/>
       <c r="C73" s="37" t="s">
@@ -2117,7 +2111,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74" s="40"/>
       <c r="B74" s="40" t="s">
         <v>115</v>
@@ -2132,7 +2126,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" s="40"/>
       <c r="B75" s="40"/>
       <c r="C75" s="37" t="s">
@@ -2145,7 +2139,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76" s="44" t="s">
         <v>116</v>
       </c>
@@ -2162,7 +2156,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77" s="48" t="s">
         <v>120</v>
       </c>
@@ -2179,7 +2173,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78" s="48" t="s">
         <v>122</v>
       </c>
@@ -2196,7 +2190,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79" s="49"/>
       <c r="B79" s="49" t="s">
         <v>124</v>
@@ -2211,7 +2205,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80" s="49"/>
       <c r="B80" s="49" t="s">
         <v>125</v>
@@ -2226,7 +2220,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81" s="49"/>
       <c r="B81" s="45" t="s">
         <v>126</v>
@@ -2241,7 +2235,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82" s="49"/>
       <c r="B82" s="49"/>
       <c r="C82" s="46" t="s">
@@ -2254,7 +2248,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83" s="49"/>
       <c r="B83" s="49" t="s">
         <v>128</v>
@@ -2269,7 +2263,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="A84" s="49"/>
       <c r="B84" s="49"/>
       <c r="C84" s="46" t="s">
@@ -2282,7 +2276,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5">
       <c r="A85" s="49"/>
       <c r="B85" s="49" t="s">
         <v>129</v>
@@ -2297,7 +2291,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86" s="49"/>
       <c r="B86" s="49"/>
       <c r="C86" s="46" t="s">
@@ -2310,7 +2304,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5">
       <c r="A87" s="49"/>
       <c r="B87" s="49" t="s">
         <v>130</v>
@@ -2325,7 +2319,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88" s="49"/>
       <c r="B88" s="49"/>
       <c r="C88" s="46" t="s">
@@ -2338,7 +2332,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89" s="50"/>
       <c r="B89" s="49" t="s">
         <v>131</v>
@@ -2353,7 +2347,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90" s="50"/>
       <c r="B90" s="52"/>
       <c r="C90" s="47" t="s">
@@ -2366,7 +2360,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91" s="49"/>
       <c r="B91" s="45" t="s">
         <v>133</v>
@@ -2381,7 +2375,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92" s="49"/>
       <c r="B92" s="49"/>
       <c r="C92" s="46" t="s">
@@ -2394,7 +2388,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5">
       <c r="A93" s="49"/>
       <c r="B93" s="49" t="s">
         <v>136</v>
@@ -2409,7 +2403,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5">
       <c r="A94" s="54"/>
       <c r="B94" s="52"/>
       <c r="C94" s="47" t="s">
@@ -2428,26 +2422,14 @@
     <mergeCell ref="A2:E3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E62" r:id="rId1"/>
-    <hyperlink ref="E37" r:id="rId2"/>
-    <hyperlink ref="E63" r:id="rId3"/>
-    <hyperlink ref="E89" r:id="rId4" display="http://www.housing.gov.ie/search/sub-topic/statistics-fire-service-activities"/>
-    <hyperlink ref="E91" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="E90" r:id="rId7" display="http://www.housing.gov.ie/search/sub-topic/statistics-fire-service-activities"/>
+    <hyperlink ref="E62" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E37" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E63" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E89" r:id="rId4" display="http://www.housing.gov.ie/search/sub-topic/statistics-fire-service-activities" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E91" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E90" r:id="rId7" display="http://www.housing.gov.ie/search/sub-topic/statistics-fire-service-activities" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2671,37 +2653,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B69E573C-BC4E-4D15-84D2-6251D1E06286}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B69E573C-BC4E-4D15-84D2-6251D1E06286}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C713A81-E0B9-40DF-A73C-E7661C5F0D8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="edfacf83-951b-4dc6-822b-2c02bca35ad8"/>
-    <ds:schemaRef ds:uri="06e0d976-3d31-4bf3-b229-12f0909620f9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C713A81-E0B9-40DF-A73C-E7661C5F0D8A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40C81BF0-49E3-4BCD-AB98-1A930086F9A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40C81BF0-49E3-4BCD-AB98-1A930086F9A5}"/>
 </file>
</xml_diff>

<commit_message>
add households and residents charts
</commit_message>
<xml_diff>
--- a/Cork_Dashboard_Indicator_List.xlsx
+++ b/Cork_Dashboard_Indicator_List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="2"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="258">
   <si>
     <t>Checklist for Cork indicators*</t>
   </si>
@@ -840,6 +840,24 @@
   </si>
   <si>
     <t>See issue https://github.com/BuildingCityDashboards/bcd-dd-v2.1/issues/1325</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>/themes#economy</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=raa01</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=BRA08&amp;PLanguage=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/themes#economy </t>
+  </si>
+  <si>
+    <t>Issue #18 - Updated to active table https://www.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=QLF08&amp;PLanguage=0</t>
   </si>
 </sst>
 </file>
@@ -967,7 +985,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1007,6 +1025,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1147,64 +1177,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1275,6 +1249,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1556,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1568,1360 +1608,1564 @@
     <col min="2" max="2" width="85.1640625" customWidth="1"/>
     <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="211.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="130" style="2" customWidth="1"/>
+    <col min="6" max="6" width="100" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-    </row>
-    <row r="2" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="77" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-    </row>
-    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="78"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-    </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="F4" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" s="31"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="85" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="F5" s="85" t="s">
+        <v>257</v>
+      </c>
+      <c r="G5" s="85" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="36"/>
+      <c r="B8" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="33" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="10" t="s">
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="37"/>
+      <c r="B9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10" t="s">
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="37"/>
+      <c r="B10" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10" t="s">
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="37"/>
+      <c r="B11" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="33" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10" t="s">
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="37"/>
+      <c r="B12" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="81" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="10" t="s">
+      <c r="F12" s="81" t="s">
+        <v>254</v>
+      </c>
+      <c r="G12" s="83" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="38"/>
+      <c r="B13" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="38"/>
+      <c r="B14" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="D14" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10" t="s">
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="38"/>
+      <c r="B15" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="33" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10" t="s">
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="38"/>
+      <c r="B16" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="D16" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="81" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12" t="s">
+      <c r="F16" s="81" t="s">
+        <v>255</v>
+      </c>
+      <c r="G16" s="83" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="38"/>
+      <c r="B17" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="D17" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="16" t="s">
+      <c r="D18" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="76" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="53"/>
+      <c r="C19" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="16" t="s">
+      <c r="D19" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="76" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="16" t="s">
+      <c r="D20" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="76" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14" t="s">
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="41"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="16" t="s">
+      <c r="D21" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="76" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14" t="s">
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="41"/>
+      <c r="B22" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="76" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14" t="s">
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="41"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="76" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14" t="s">
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="41"/>
+      <c r="B24" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="76" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14" t="s">
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="41"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="76" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14" t="s">
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="41"/>
+      <c r="B26" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="19" t="s">
+      <c r="D26" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="51" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14" t="s">
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="41"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="19" t="s">
+      <c r="D27" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="51" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14" t="s">
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="41"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="19" t="s">
+      <c r="D28" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="51" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14" t="s">
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="41"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="19" t="s">
+      <c r="D29" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="51" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14" t="s">
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="41"/>
+      <c r="B30" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="76" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14" t="s">
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="41"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="76" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14" t="s">
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="41"/>
+      <c r="B32" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="19" t="s">
+      <c r="D32" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="51" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="21" t="s">
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="41"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="19" t="s">
+      <c r="D33" s="79" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="51" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="25" t="s">
+      <c r="D34" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="45" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="25" t="s">
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="47"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="25" t="s">
+      <c r="D35" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="45" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27" t="s">
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="47"/>
+      <c r="B36" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="25" t="s">
+      <c r="D36" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="45" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="25" t="s">
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="25" t="s">
+      <c r="D37" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="45" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27" t="s">
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="47"/>
+      <c r="B38" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="25" t="s">
+      <c r="D38" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="45" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="25" t="s">
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="47"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="25" t="s">
+      <c r="D39" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="45" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="27"/>
-      <c r="B40" s="27" t="s">
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="47"/>
+      <c r="B40" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="25" t="s">
+      <c r="D40" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="45" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="25" t="s">
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="25" t="s">
+      <c r="D41" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="45" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27" t="s">
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="47"/>
+      <c r="B42" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="25" t="s">
+      <c r="D42" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="45" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="25" t="s">
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="47"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="25" t="s">
+      <c r="D43" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="45" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27" t="s">
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="47"/>
+      <c r="B44" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="25" t="s">
+      <c r="D44" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="45" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="25" t="s">
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="47"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="25" t="s">
+      <c r="D45" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="45" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28" t="s">
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="25" t="s">
+      <c r="D46" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="45" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27" t="s">
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="47"/>
+      <c r="B47" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="D47" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="25" t="s">
+      <c r="D47" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="45" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27" t="s">
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="47"/>
+      <c r="B48" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="D48" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="25" t="s">
+      <c r="D48" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="45" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="27"/>
-      <c r="B49" s="27" t="s">
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="47"/>
+      <c r="B49" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="25" t="s">
+      <c r="D49" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="45" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="27"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="25" t="s">
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="47"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D50" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="25" t="s">
+      <c r="D50" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="45" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="29" t="s">
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="C51" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="31" t="s">
+      <c r="D51" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="51" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="33"/>
-      <c r="B52" s="33" t="s">
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="53"/>
+      <c r="B52" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="31" t="s">
+      <c r="C52" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D52" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="31" t="s">
+      <c r="D52" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="51" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="33"/>
-      <c r="B53" s="33" t="s">
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="53"/>
+      <c r="B53" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="31" t="s">
+      <c r="C53" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D53" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="31" t="s">
+      <c r="D53" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="51" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33" t="s">
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="53"/>
+      <c r="B54" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="31" t="s">
+      <c r="C54" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="31" t="s">
+      <c r="D54" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="51" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="33"/>
-      <c r="B55" s="33" t="s">
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="53"/>
+      <c r="B55" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="31" t="s">
+      <c r="C55" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D55" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="31" t="s">
+      <c r="D55" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="51" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="33"/>
-      <c r="B56" s="33" t="s">
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="53"/>
+      <c r="B56" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="31" t="s">
+      <c r="C56" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D56" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="31" t="s">
+      <c r="D56" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="51" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="33"/>
-      <c r="B57" s="30" t="s">
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="53"/>
+      <c r="B57" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="31" t="s">
+      <c r="C57" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D57" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="31" t="s">
+      <c r="D57" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="51" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="34"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="31" t="s">
+      <c r="F57" s="31"/>
+      <c r="G57" s="31"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="54"/>
+      <c r="B58" s="54"/>
+      <c r="C58" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="D58" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="31" t="s">
+      <c r="D58" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="51" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="33"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="31" t="s">
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="53"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="31" t="s">
+      <c r="D59" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="51" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="33"/>
-      <c r="B60" s="33" t="s">
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="53"/>
+      <c r="B60" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="C60" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="D60" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="31" t="s">
+      <c r="D60" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="51" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="33"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="31" t="s">
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="53"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="D61" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="31" t="s">
+      <c r="D61" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="51" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="35" t="s">
+      <c r="F61" s="31"/>
+      <c r="G61" s="31"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="B62" s="36" t="s">
+      <c r="B62" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="C62" s="37" t="s">
+      <c r="C62" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="D62" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="37" t="s">
+      <c r="D62" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="57" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="39" t="s">
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="B63" s="40"/>
-      <c r="C63" s="37" t="s">
+      <c r="B63" s="60"/>
+      <c r="C63" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="D63" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="41" t="s">
+      <c r="D63" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="57" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="42"/>
-      <c r="B64" s="40" t="s">
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="61"/>
+      <c r="B64" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="C64" s="37" t="s">
+      <c r="C64" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D64" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="37" t="s">
+      <c r="D64" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="57" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="42"/>
-      <c r="B65" s="41"/>
-      <c r="C65" s="37" t="s">
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="61"/>
+      <c r="B65" s="62"/>
+      <c r="C65" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D65" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="37" t="s">
+      <c r="D65" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="57" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="40"/>
-      <c r="B66" s="36" t="s">
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="60"/>
+      <c r="B66" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="C66" s="37" t="s">
+      <c r="C66" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="37" t="s">
+      <c r="D66" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="40"/>
-      <c r="B67" s="40"/>
-      <c r="C67" s="37" t="s">
+      <c r="F66" s="31"/>
+      <c r="G66" s="31"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="60"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D67" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="37" t="s">
+      <c r="D67" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="40"/>
-      <c r="B68" s="40" t="s">
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="60"/>
+      <c r="B68" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="C68" s="37" t="s">
+      <c r="C68" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D68" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="37" t="s">
+      <c r="D68" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="40"/>
-      <c r="B69" s="40"/>
-      <c r="C69" s="37" t="s">
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="60"/>
+      <c r="B69" s="60"/>
+      <c r="C69" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D69" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="37" t="s">
+      <c r="D69" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="40"/>
-      <c r="B70" s="40" t="s">
+      <c r="F69" s="31"/>
+      <c r="G69" s="31"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="60"/>
+      <c r="B70" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C70" s="37" t="s">
+      <c r="C70" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D70" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="37" t="s">
+      <c r="D70" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="40"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="37" t="s">
+      <c r="F70" s="31"/>
+      <c r="G70" s="31"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="60"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D71" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="37" t="s">
+      <c r="D71" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="40"/>
-      <c r="B72" s="40" t="s">
+      <c r="F71" s="31"/>
+      <c r="G71" s="31"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="60"/>
+      <c r="B72" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="C72" s="37" t="s">
+      <c r="C72" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D72" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="37" t="s">
+      <c r="D72" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="57" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="40"/>
-      <c r="B73" s="40"/>
-      <c r="C73" s="37" t="s">
+      <c r="F72" s="31"/>
+      <c r="G72" s="31"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="60"/>
+      <c r="B73" s="60"/>
+      <c r="C73" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="37" t="s">
+      <c r="D73" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="57" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="40"/>
-      <c r="B74" s="40" t="s">
+      <c r="F73" s="31"/>
+      <c r="G73" s="31"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="60"/>
+      <c r="B74" s="60" t="s">
         <v>115</v>
       </c>
-      <c r="C74" s="37" t="s">
+      <c r="C74" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D74" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="37" t="s">
+      <c r="D74" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="40"/>
-      <c r="B75" s="40"/>
-      <c r="C75" s="37" t="s">
+      <c r="F74" s="31"/>
+      <c r="G74" s="31"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="60"/>
+      <c r="B75" s="60"/>
+      <c r="C75" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D75" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="37" t="s">
+      <c r="D75" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="44" t="s">
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="B76" s="45" t="s">
+      <c r="B76" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="C76" s="46" t="s">
+      <c r="C76" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="D76" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="46" t="s">
+      <c r="D76" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="66" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="48" t="s">
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="B77" s="49" t="s">
+      <c r="B77" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="C77" s="46" t="s">
+      <c r="C77" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="D77" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" s="46" t="s">
+      <c r="D77" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="66" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="48" t="s">
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="B78" s="49" t="s">
+      <c r="B78" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="C78" s="46" t="s">
+      <c r="C78" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="D78" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="46" t="s">
+      <c r="D78" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="66" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="49"/>
-      <c r="B79" s="49" t="s">
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="69"/>
+      <c r="B79" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="C79" s="46" t="s">
+      <c r="C79" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="D79" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" s="46" t="s">
+      <c r="D79" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="66" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="49"/>
-      <c r="B80" s="49" t="s">
+      <c r="F79" s="31"/>
+      <c r="G79" s="31"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="69"/>
+      <c r="B80" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="C80" s="46" t="s">
+      <c r="C80" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="D80" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="46" t="s">
+      <c r="D80" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="66" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="49"/>
-      <c r="B81" s="45" t="s">
+      <c r="F80" s="31"/>
+      <c r="G80" s="31"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="69"/>
+      <c r="B81" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="C81" s="46" t="s">
+      <c r="C81" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D81" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" s="46" t="s">
+      <c r="D81" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="66" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="49"/>
-      <c r="B82" s="49"/>
-      <c r="C82" s="46" t="s">
+      <c r="F81" s="31"/>
+      <c r="G81" s="31"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="69"/>
+      <c r="B82" s="69"/>
+      <c r="C82" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="D82" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="46" t="s">
+      <c r="D82" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="66" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="49"/>
-      <c r="B83" s="49" t="s">
+      <c r="F82" s="31"/>
+      <c r="G82" s="31"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="69"/>
+      <c r="B83" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="C83" s="46" t="s">
+      <c r="C83" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D83" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" s="46" t="s">
+      <c r="D83" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="66" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="49"/>
-      <c r="B84" s="49"/>
-      <c r="C84" s="46" t="s">
+      <c r="F83" s="31"/>
+      <c r="G83" s="31"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="69"/>
+      <c r="B84" s="69"/>
+      <c r="C84" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="D84" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="46" t="s">
+      <c r="D84" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="66" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="49"/>
-      <c r="B85" s="49" t="s">
+      <c r="F84" s="31"/>
+      <c r="G84" s="31"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="69"/>
+      <c r="B85" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="C85" s="46" t="s">
+      <c r="C85" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D85" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" s="46" t="s">
+      <c r="D85" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="66" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="49"/>
-      <c r="B86" s="49"/>
-      <c r="C86" s="46" t="s">
+      <c r="F85" s="31"/>
+      <c r="G85" s="31"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="69"/>
+      <c r="B86" s="69"/>
+      <c r="C86" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="D86" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E86" s="46" t="s">
+      <c r="D86" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="66" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="49"/>
-      <c r="B87" s="49" t="s">
+      <c r="F86" s="31"/>
+      <c r="G86" s="31"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="69"/>
+      <c r="B87" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="C87" s="46" t="s">
+      <c r="C87" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D87" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E87" s="46" t="s">
+      <c r="D87" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="66" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="49"/>
-      <c r="B88" s="49"/>
-      <c r="C88" s="46" t="s">
+      <c r="F87" s="31"/>
+      <c r="G87" s="31"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="69"/>
+      <c r="B88" s="69"/>
+      <c r="C88" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="D88" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E88" s="46" t="s">
+      <c r="D88" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" s="66" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="50"/>
-      <c r="B89" s="49" t="s">
+      <c r="F88" s="31"/>
+      <c r="G88" s="31"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="70"/>
+      <c r="B89" s="69" t="s">
         <v>131</v>
       </c>
-      <c r="C89" s="50" t="s">
+      <c r="C89" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="D89" s="46" t="s">
+      <c r="D89" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="E89" s="51" t="s">
+      <c r="E89" s="71" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="50"/>
-      <c r="B90" s="52"/>
-      <c r="C90" s="47" t="s">
+      <c r="F89" s="31"/>
+      <c r="G89" s="31"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="70"/>
+      <c r="B90" s="72"/>
+      <c r="C90" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="D90" s="53" t="s">
+      <c r="D90" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="E90" s="51" t="s">
+      <c r="E90" s="71" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="49"/>
-      <c r="B91" s="45" t="s">
+      <c r="F90" s="31"/>
+      <c r="G90" s="31"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="69"/>
+      <c r="B91" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="C91" s="46" t="s">
+      <c r="C91" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="D91" s="47" t="s">
+      <c r="D91" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="E91" s="52" t="s">
+      <c r="E91" s="66" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="49"/>
-      <c r="B92" s="49"/>
-      <c r="C92" s="46" t="s">
+      <c r="F91" s="31"/>
+      <c r="G91" s="31"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="69"/>
+      <c r="B92" s="69"/>
+      <c r="C92" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="D92" s="47" t="s">
+      <c r="D92" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="E92" s="46" t="s">
+      <c r="E92" s="66" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="49"/>
-      <c r="B93" s="49" t="s">
+      <c r="F92" s="31"/>
+      <c r="G92" s="31"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="69"/>
+      <c r="B93" s="69" t="s">
         <v>136</v>
       </c>
-      <c r="C93" s="46" t="s">
+      <c r="C93" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="D93" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E93" s="46" t="s">
+      <c r="D93" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93" s="66" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="54"/>
-      <c r="B94" s="52"/>
-      <c r="C94" s="47" t="s">
+      <c r="F93" s="31"/>
+      <c r="G93" s="31"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="74"/>
+      <c r="B94" s="72"/>
+      <c r="C94" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="D94" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="E94" s="46" t="s">
+      <c r="D94" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94" s="66" t="s">
         <v>135</v>
       </c>
+      <c r="F94" s="31"/>
+      <c r="G94" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2938,6 +3182,7 @@
     <hyperlink ref="E90" r:id="rId7" display="http://www.housing.gov.ie/search/sub-topic/statistics-fire-service-activities"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2957,887 +3202,887 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="39.83203125" style="59" customWidth="1"/>
-    <col min="3" max="3" width="62.6640625" style="59" customWidth="1"/>
-    <col min="4" max="4" width="60.1640625" style="59" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" style="59" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="59"/>
-    <col min="7" max="7" width="160.6640625" style="59" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="59"/>
+    <col min="1" max="2" width="39.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="7" max="7" width="160.6640625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="58"/>
-      <c r="B1" s="59" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="5" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="21" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="61"/>
-      <c r="B13" s="66" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="D14" s="61">
+      <c r="D14" s="7">
         <v>2012</v>
       </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="60">
+      <c r="D15" s="6">
         <v>2013</v>
       </c>
-      <c r="E15" s="60"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="61"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="61"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="61"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="61"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="13" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="42" x14ac:dyDescent="0.2">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C20" s="59" t="s">
+      <c r="C20" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="58" t="s">
+      <c r="A23" s="4" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="12" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C25" s="66" t="s">
+      <c r="C25" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D25" s="59" t="s">
+      <c r="D25" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="59" t="s">
+      <c r="A26" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D26" s="59" t="s">
+      <c r="D26" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="28" x14ac:dyDescent="0.2">
-      <c r="A27" s="59" t="s">
+      <c r="A27" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D27" s="59" t="s">
+      <c r="D27" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E27" s="59" t="s">
+      <c r="E27" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="28" x14ac:dyDescent="0.2">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D28" s="59" t="s">
+      <c r="D28" s="5" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="28" x14ac:dyDescent="0.2">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="12" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="28" x14ac:dyDescent="0.2">
-      <c r="A30" s="59" t="s">
+      <c r="A30" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="12" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C31" s="72" t="s">
+      <c r="C31" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="D31" s="71" t="s">
+      <c r="D31" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="E31" s="71"/>
+      <c r="E31" s="17"/>
     </row>
     <row r="32" spans="1:10" ht="28" x14ac:dyDescent="0.2">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D32" s="59" t="s">
+      <c r="D32" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="E32" s="59" t="s">
+      <c r="E32" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="D33" s="59" t="s">
+      <c r="D33" s="5" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A34" s="59" t="s">
+      <c r="A34" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B34" s="62" t="s">
+      <c r="B34" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C34" s="66" t="s">
+      <c r="C34" s="12" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A35" s="59" t="s">
+      <c r="A35" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D35" s="59" t="s">
+      <c r="D35" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="4" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="66" t="s">
+      <c r="B38" s="12" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="59" t="s">
+      <c r="A39" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B39" s="62" t="s">
+      <c r="B39" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E39" s="59" t="s">
+      <c r="E39" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="59" t="s">
+      <c r="A40" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B40" s="62" t="s">
+      <c r="B40" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="D40" s="59" t="s">
+      <c r="D40" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E40" s="59" t="s">
+      <c r="E40" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="59" t="s">
+      <c r="A41" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B41" s="62" t="s">
+      <c r="B41" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="D41" s="59" t="s">
+      <c r="D41" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E41" s="59" t="s">
+      <c r="E41" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="59" t="s">
+      <c r="A42" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="D42" s="59" t="s">
+      <c r="D42" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E42" s="59" t="s">
+      <c r="E42" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="59" t="s">
+      <c r="A43" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B43" s="62" t="s">
+      <c r="B43" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="59" t="s">
+      <c r="D43" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E43" s="59" t="s">
+      <c r="E43" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B44" s="62" t="s">
+      <c r="B44" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C44" s="66" t="s">
+      <c r="C44" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="D44" s="59" t="s">
+      <c r="D44" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E44" s="59" t="s">
+      <c r="E44" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="59" t="s">
+      <c r="A45" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E45" s="59" t="s">
+      <c r="E45" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A46" s="59" t="s">
+      <c r="A46" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C46" s="66" t="s">
+      <c r="C46" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="E46" s="59" t="s">
+      <c r="E46" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A47" s="59" t="s">
+      <c r="A47" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B47" s="62" t="s">
+      <c r="B47" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C47" s="66" t="s">
+      <c r="C47" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="D47" s="59" t="s">
+      <c r="D47" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E47" s="59" t="s">
+      <c r="E47" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="59" t="s">
+      <c r="A48" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B48" s="62" t="s">
+      <c r="B48" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C48" s="66" t="s">
+      <c r="C48" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="D48" s="59" t="s">
+      <c r="D48" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E48" s="59" t="s">
+      <c r="E48" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A49" s="59" t="s">
+      <c r="A49" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B49" s="62" t="s">
+      <c r="B49" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C49" s="66" t="s">
+      <c r="C49" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D49" s="59" t="s">
+      <c r="D49" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="66" t="s">
+      <c r="B51" s="12" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A52" s="59" t="s">
+      <c r="A52" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B52" s="62" t="s">
+      <c r="B52" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C52" s="66" t="s">
+      <c r="C52" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="66" t="s">
+      <c r="D52" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="E52" s="59" t="s">
+      <c r="E52" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A53" s="59" t="s">
+      <c r="A53" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B53" s="62" t="s">
+      <c r="B53" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C53" s="66" t="s">
+      <c r="C53" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="66"/>
-      <c r="E53" s="59" t="s">
+      <c r="D53" s="12"/>
+      <c r="E53" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A54" s="59" t="s">
+      <c r="A54" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B54" s="62" t="s">
+      <c r="B54" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C54" s="59" t="s">
+      <c r="C54" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E54" s="59" t="s">
+      <c r="E54" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="42" x14ac:dyDescent="0.2">
-      <c r="A55" s="59" t="s">
+      <c r="A55" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="62" t="s">
+      <c r="B55" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C55" s="66" t="s">
+      <c r="C55" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="E55" s="73" t="s">
+      <c r="E55" s="19" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="62" t="s">
+      <c r="B56" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C56" s="66" t="s">
+      <c r="C56" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="D56" s="59" t="s">
+      <c r="D56" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="E56" s="73" t="s">
+      <c r="E56" s="19" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A57" s="59" t="s">
+      <c r="A57" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B57" s="62" t="s">
+      <c r="B57" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C57" s="59" t="s">
+      <c r="C57" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D57" s="59" t="s">
+      <c r="D57" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E57" s="73" t="s">
+      <c r="E57" s="19" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="59" t="s">
+      <c r="A59" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="B59" s="59" t="s">
+      <c r="B59" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="C59" s="59" t="s">
+      <c r="C59" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="D59" s="59" t="s">
+      <c r="D59" s="5" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="58" t="s">
+      <c r="A60" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="42" x14ac:dyDescent="0.2">
-      <c r="A61" s="74" t="s">
+      <c r="A61" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="B61" s="59" t="s">
+      <c r="B61" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C61" s="57" t="s">
+      <c r="C61" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D61" s="59" t="s">
+      <c r="D61" s="5" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A62" s="74" t="s">
+      <c r="A62" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="B62" s="59" t="s">
+      <c r="B62" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C62" s="57" t="s">
+      <c r="C62" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D62" s="59" t="s">
+      <c r="D62" s="5" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A63" s="74" t="s">
+      <c r="A63" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="B63" s="59" t="s">
+      <c r="B63" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C63" s="57" t="s">
+      <c r="C63" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D63" s="59">
+      <c r="D63" s="5">
         <v>2014</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A64" s="74" t="s">
+      <c r="A64" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="B64" s="59" t="s">
+      <c r="B64" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C64" s="57" t="s">
+      <c r="C64" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D64" s="59">
+      <c r="D64" s="5">
         <v>2013</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A65" s="56" t="s">
+      <c r="A65" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B65" s="59" t="s">
+      <c r="B65" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D65" s="59">
+      <c r="D65" s="5">
         <v>2011</v>
       </c>
-      <c r="E65" s="59" t="s">
+      <c r="E65" s="5" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="58" t="s">
+      <c r="A68" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B68" s="66" t="s">
+      <c r="B68" s="12" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A69" s="56" t="s">
+      <c r="A69" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B69" s="59" t="s">
+      <c r="B69" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C69" s="57" t="s">
+      <c r="C69" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D69" s="59" t="s">
+      <c r="D69" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A70" s="56" t="s">
+      <c r="A70" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B70" s="59" t="s">
+      <c r="B70" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C70" s="57" t="s">
+      <c r="C70" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D70" s="56" t="s">
+      <c r="D70" s="2" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A71" s="56" t="s">
+      <c r="A71" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B71" s="59" t="s">
+      <c r="B71" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C71" s="57" t="s">
+      <c r="C71" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D71" s="59" t="s">
+      <c r="D71" s="5" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A72" s="56" t="s">
+      <c r="A72" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B72" s="59" t="s">
+      <c r="B72" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C72" s="57" t="s">
+      <c r="C72" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D72" s="59" t="s">
+      <c r="D72" s="5" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="56" t="s">
+      <c r="A73" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B73" s="59" t="s">
+      <c r="B73" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C73" s="57" t="s">
+      <c r="C73" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D73" s="59" t="s">
+      <c r="D73" s="5" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A74" s="56" t="s">
+      <c r="A74" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B74" s="59" t="s">
+      <c r="B74" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C74" s="57" t="s">
+      <c r="C74" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D74" s="59" t="s">
+      <c r="D74" s="5" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A75" s="56" t="s">
+      <c r="A75" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B75" s="73" t="s">
+      <c r="B75" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="C75" s="57" t="s">
+      <c r="C75" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D75" s="73" t="s">
+      <c r="D75" s="19" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3954,7 +4199,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="1" t="s">
         <v>246</v>
       </c>
     </row>

</xml_diff>